<commit_message>
Finished formatting resurface text
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,24 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>rink</t>
-  </si>
-  <si>
-    <t>5/11/2017</t>
-  </si>
-  <si>
-    <t>11:25PM</t>
-  </si>
-  <si>
-    <t>edged</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Rink</t>
+  </si>
+  <si>
+    <t>Board Brush</t>
+  </si>
+  <si>
+    <t>Wet Cut</t>
+  </si>
+  <si>
+    <t>Dry Cut</t>
+  </si>
+  <si>
+    <t>Edged</t>
   </si>
   <si>
     <t>Three Lap</t>
@@ -41,6 +44,42 @@
   </si>
   <si>
     <t>Center Flood</t>
+  </si>
+  <si>
+    <t>Dump Tank</t>
+  </si>
+  <si>
+    <t>HoneyWells</t>
+  </si>
+  <si>
+    <t>Room Temp/Humidity</t>
+  </si>
+  <si>
+    <t>Initials</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>5/15/2017</t>
+  </si>
+  <si>
+    <t>6:50PM</t>
+  </si>
+  <si>
+    <t>Rink1</t>
+  </si>
+  <si>
+    <t>Brush</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>6:51PM</t>
   </si>
 </sst>
 </file>
@@ -372,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,39 +427,105 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="N3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" t="s">
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" t="s">
-        <v>6</v>
+      <c r="J3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>